<commit_message>
shivam changes added config and Login TIme Script
</commit_message>
<xml_diff>
--- a/umang/TestSuite/TestSuite.xlsx
+++ b/umang/TestSuite/TestSuite.xlsx
@@ -479,8 +479,8 @@
   </sheetPr>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>